<commit_message>
updated excel action recognition
</commit_message>
<xml_diff>
--- a/Documents/Scenes_ExcelSheet.xlsx
+++ b/Documents/Scenes_ExcelSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jiss\Amrita\SecondSem\ComputerVision\CaseStudy\LaneDetection\lane_detection\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78C58E4-24FE-4F07-960F-C46A28C3BE9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496D0F1B-21B4-4489-A815-CC5A273E419E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" xr2:uid="{92E58B98-A324-43E6-A747-6F6A67D8FE0B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Frame Number</t>
   </si>
@@ -190,6 +190,33 @@
   </si>
   <si>
     <t>Road Based on Lane Marking Visibility</t>
+  </si>
+  <si>
+    <t>Object Dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Face Detection </t>
+  </si>
+  <si>
+    <t>FD Algorithm</t>
+  </si>
+  <si>
+    <t>FD Dataset Name</t>
+  </si>
+  <si>
+    <t>Optical flow algorithm</t>
+  </si>
+  <si>
+    <t>Action Recognition</t>
+  </si>
+  <si>
+    <t>Action Dataset</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Deep Learning Arch. Name</t>
   </si>
 </sst>
 </file>
@@ -402,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -418,12 +445,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -453,6 +474,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -466,6 +493,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -782,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D735AB2F-45E7-48F6-AF4F-8EFA3210DCB8}">
-  <dimension ref="A2:S36"/>
+  <dimension ref="A2:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="S2" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,9 +827,17 @@
     <col min="17" max="17" width="35.140625" customWidth="1"/>
     <col min="18" max="18" width="50.140625" customWidth="1"/>
     <col min="19" max="19" width="54.5703125" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" customWidth="1"/>
+    <col min="22" max="22" width="21.140625" customWidth="1"/>
+    <col min="23" max="23" width="17" customWidth="1"/>
+    <col min="24" max="24" width="23.140625" customWidth="1"/>
+    <col min="25" max="25" width="22.5703125" customWidth="1"/>
+    <col min="26" max="26" width="18.85546875" customWidth="1"/>
+    <col min="27" max="27" width="24.5703125" customWidth="1"/>
+    <col min="28" max="28" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
         <v>21</v>
       </c>
@@ -817,7 +855,7 @@
       <c r="N2" s="29"/>
       <c r="O2" s="30"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="28" t="s">
         <v>22</v>
@@ -836,28 +874,49 @@
       <c r="N3" s="31"/>
       <c r="O3" s="32"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10" t="s">
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="13"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="11"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z4" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA4" s="33"/>
+      <c r="AB4" s="33"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="7" t="s">
         <v>0</v>
@@ -901,8 +960,23 @@
       <c r="O5" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
@@ -921,7 +995,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
         <v>3</v>
@@ -940,7 +1014,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -959,7 +1033,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
@@ -977,7 +1051,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1007,154 +1081,155 @@
       </c>
     </row>
     <row r="21" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q21" s="25" t="s">
+      <c r="Q21" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="R21" s="18" t="s">
+      <c r="R21" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="S21" s="17" t="s">
+      <c r="S21" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q22" s="27"/>
-      <c r="R22" s="14" t="s">
+      <c r="Q22" s="25"/>
+      <c r="R22" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="S22" s="11" t="s">
+      <c r="S22" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q23" s="26"/>
-      <c r="R23" s="14" t="s">
+      <c r="Q23" s="24"/>
+      <c r="R23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="S23" s="13" t="s">
+      <c r="S23" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q24" s="22"/>
-      <c r="R24" s="24"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="22"/>
       <c r="S24" s="4"/>
     </row>
     <row r="25" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q25" s="25" t="s">
+      <c r="Q25" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="R25" s="21" t="s">
+      <c r="R25" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="S25" s="17" t="s">
+      <c r="S25" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q26" s="26"/>
-      <c r="R26" s="14" t="s">
+      <c r="Q26" s="24"/>
+      <c r="R26" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="S26" s="13" t="s">
+      <c r="S26" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="27" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q27" s="19"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="11"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="9"/>
     </row>
     <row r="28" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q28" s="25" t="s">
+      <c r="Q28" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="R28" s="14" t="s">
+      <c r="R28" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="S28" s="17" t="s">
+      <c r="S28" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="29" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q29" s="27"/>
-      <c r="R29" s="14" t="s">
+      <c r="Q29" s="25"/>
+      <c r="R29" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="S29" s="11" t="s">
+      <c r="S29" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="30" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q30" s="26"/>
-      <c r="R30" s="14" t="s">
+      <c r="Q30" s="24"/>
+      <c r="R30" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="S30" s="13" t="s">
+      <c r="S30" s="11" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q31" s="19"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="11"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="22"/>
+      <c r="S31" s="9"/>
     </row>
     <row r="32" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q32" s="25" t="s">
+      <c r="Q32" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="R32" s="14" t="s">
+      <c r="R32" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="S32" s="17" t="s">
+      <c r="S32" s="15" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="33" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q33" s="26"/>
-      <c r="R33" s="15" t="s">
+      <c r="Q33" s="24"/>
+      <c r="R33" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="S33" s="13" t="s">
+      <c r="S33" s="11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q34" s="16"/>
-      <c r="R34" s="23"/>
-      <c r="S34" s="17"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="15"/>
     </row>
     <row r="35" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q35" s="25" t="s">
+      <c r="Q35" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="R35" s="18" t="s">
+      <c r="R35" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="S35" s="17" t="s">
+      <c r="S35" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="36" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q36" s="26"/>
-      <c r="R36" s="15" t="s">
+      <c r="Q36" s="24"/>
+      <c r="R36" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="S36" s="13" t="s">
+      <c r="S36" s="11" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="Q21:Q23"/>
+    <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="Q35:Q36"/>
     <mergeCell ref="Q28:Q30"/>
     <mergeCell ref="Q32:Q33"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I4:L4"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="B3:O3"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="Q21:Q23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>